<commit_message>
added functionality of table output of vacancies
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -450,9 +450,9 @@
   <cols>
     <col width="6" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="28" customWidth="1" min="3" max="3"/>
+    <col width="29" customWidth="1" min="3" max="3"/>
     <col width="21" customWidth="1" min="4" max="4"/>
-    <col width="31" customWidth="1" min="5" max="5"/>
+    <col width="32" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -468,7 +468,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Средняя зарплата - инженер</t>
+          <t>Средняя зарплата - водитель</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -478,7 +478,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Количество вакансий - инженер</t>
+          <t>Количество вакансий - водитель</t>
         </is>
       </c>
     </row>
@@ -490,13 +490,13 @@
         <v>38916</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>36592</v>
+        <v>56419</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>2196</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>69</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3">
@@ -507,13 +507,13 @@
         <v>43646</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>40577</v>
+        <v>65786</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>17549</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>571</v>
+        <v>696</v>
       </c>
     </row>
     <row r="4">
@@ -524,13 +524,13 @@
         <v>42492</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>39267</v>
+        <v>64078</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>17709</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>447</v>
+        <v>792</v>
       </c>
     </row>
     <row r="5">
@@ -541,13 +541,13 @@
         <v>43846</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>36541</v>
+        <v>66416</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>29093</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>975</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="6">
@@ -558,13 +558,13 @@
         <v>47451</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>42315</v>
+        <v>73525</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>36700</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>984</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="7">
@@ -575,13 +575,13 @@
         <v>48243</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>45573</v>
+        <v>76036</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>44153</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>1275</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="8">
@@ -592,13 +592,13 @@
         <v>51510</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>45769</v>
+        <v>78612</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>59954</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>1800</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="9">
@@ -609,13 +609,13 @@
         <v>50658</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>48181</v>
+        <v>80402</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>66837</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>2058</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="10">
@@ -626,13 +626,13 @@
         <v>52696</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>48585</v>
+        <v>91682</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>70039</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>1615</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="11">
@@ -643,13 +643,13 @@
         <v>62675</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>51810</v>
+        <v>78512</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>75145</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>1854</v>
+        <v>2604</v>
       </c>
     </row>
     <row r="12">
@@ -660,13 +660,13 @@
         <v>60935</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>53787</v>
+        <v>93515</v>
       </c>
       <c r="D12" s="2" t="n">
         <v>82823</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>2557</v>
+        <v>2534</v>
       </c>
     </row>
     <row r="13">
@@ -677,13 +677,13 @@
         <v>58335</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>57867</v>
+        <v>95512</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>131701</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>3379</v>
+        <v>3050</v>
       </c>
     </row>
     <row r="14">
@@ -694,13 +694,13 @@
         <v>69467</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>64287</v>
+        <v>104304</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>115086</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>3808</v>
+        <v>3225</v>
       </c>
     </row>
     <row r="15">
@@ -711,13 +711,13 @@
         <v>73431</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>68126</v>
+        <v>111293</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>102243</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>3338</v>
+        <v>3123</v>
       </c>
     </row>
     <row r="16">
@@ -728,13 +728,13 @@
         <v>82690</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>76993</v>
+        <v>119943</v>
       </c>
       <c r="D16" s="2" t="n">
         <v>57623</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>1933</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="17">
@@ -745,13 +745,13 @@
         <v>91795</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>81351</v>
+        <v>142799</v>
       </c>
       <c r="D17" s="2" t="n">
         <v>18294</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>819</v>
+        <v>525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added csv file split functionality
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -450,9 +450,9 @@
   <cols>
     <col width="6" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="32" customWidth="1" min="3" max="3"/>
+    <col width="28" customWidth="1" min="3" max="3"/>
     <col width="21" customWidth="1" min="4" max="4"/>
-    <col width="35" customWidth="1" min="5" max="5"/>
+    <col width="31" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -468,7 +468,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Средняя зарплата - Программист</t>
+          <t>Средняя зарплата - Инженер</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -478,7 +478,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Количество вакансий - Программист</t>
+          <t>Количество вакансий - Инженер</t>
         </is>
       </c>
     </row>
@@ -490,13 +490,13 @@
         <v>94892</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>101666</v>
+        <v>68861</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>91</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>